<commit_message>
add employee deduction with no point to report
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplateTTCS.xlsx
+++ b/ATV_Allowance/Templates/TemplateTTCS.xlsx
@@ -311,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -437,6 +437,12 @@
     </xf>
     <xf numFmtId="41" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1160,8 +1166,8 @@
   </sheetPr>
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1411,21 +1417,21 @@
         <v>26</v>
       </c>
       <c r="C8" s="28"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="47"/>
       <c r="S8" s="23"/>
       <c r="T8" s="24"/>
     </row>
@@ -1435,21 +1441,21 @@
         <v>27</v>
       </c>
       <c r="C9" s="29"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
       <c r="S9" s="25"/>
       <c r="T9" s="22"/>
     </row>
@@ -1459,21 +1465,21 @@
         <v>28</v>
       </c>
       <c r="C10" s="29"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
       <c r="S10" s="25"/>
       <c r="T10" s="22"/>
     </row>

</xml_diff>